<commit_message>
close defect : Add incident api - applicant ritual id details and update staff main data template HAJ-1074
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/8/staff-main-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/8/staff-main-data.xlsx
@@ -69,30 +69,30 @@
 M/F</t>
   </si>
   <si>
-    <t>StaffIDNumber  
-	رقم الهوية الوطنية / الإقامة</t>
-  </si>
-  <si>
-    <t>StaffPassportNo
-	رقم الجواز</t>
-  </si>
-  <si>
-    <t>StaffDateOfBirth
-	تاريخ الميلاد
-DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t>StaffDateOfBirthHijri
-	تاريخ الميلاد بالهجري
-YYYYMMDD</t>
-  </si>
-  <si>
     <t>JobTitleCode
 	المهنة</t>
   </si>
   <si>
     <t>season
 	الموسم الهجرى</t>
+  </si>
+  <si>
+    <t>IDNumber  
+	رقم الهوية الوطنية / الإقامة</t>
+  </si>
+  <si>
+    <t>PassportNo
+	رقم الجواز</t>
+  </si>
+  <si>
+    <t>DateOfBirth
+	تاريخ الميلاد
+DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>DateOfBirthHijri
+	تاريخ الميلاد بالهجري
+YYYYMMDD</t>
   </si>
 </sst>
 </file>
@@ -684,10 +684,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:Q497" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="20% - Accent1">
   <autoFilter ref="B3:Q497"/>
   <tableColumns count="16">
-    <tableColumn id="2" name="StaffIDNumber  _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="15"/>
-    <tableColumn id="3" name="StaffPassportNo_x000a__x0009_رقم الجواز" dataDxfId="14"/>
-    <tableColumn id="7" name="StaffDateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="13"/>
-    <tableColumn id="8" name="StaffDateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="12"/>
+    <tableColumn id="2" name="IDNumber  _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="15"/>
+    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="14"/>
+    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="13"/>
+    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="12"/>
     <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="11"/>
     <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="10"/>
     <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="9"/>
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,16 +997,16 @@
   <sheetData>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>0</v>
@@ -1030,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>7</v>
@@ -1042,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -19019,11 +19019,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
+<XMLData TextToDisplay="RightsWATCHMark">4|ELM-ENG-INT|{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19031,11 +19031,11 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="RightsWATCHMark">4|ELM-ENG-INT|{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19043,13 +19043,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -19061,13 +19061,13 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>